<commit_message>
read channels (pyedflib) w/ fs
</commit_message>
<xml_diff>
--- a/log/channel/cnc_chc.xlsx
+++ b/log/channel/cnc_chc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92a996cea29e9e70/future/复旦/信息学院/课题组/narcolepsy_night/narcolepsy_night_code/log/channel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_CBB0F0A0816AD862A26FEFC06318EDE8E7C5C28F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9E21C25-F682-44B1-9E74-7ABD0BCEA954}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_EAF872967FBACC58567B142B27D06862DC7B69B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06D9D854-1C4D-4E1F-AD99-967034CA15D2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,145 +22,145 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="47">
   <si>
-    <t>chc001-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc004-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc005-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc006-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc008-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc009-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc010-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc012-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc013-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc014-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc015-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc016-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc022-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc025-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc027-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc028-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc033-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc035-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc037-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc040-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc041-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc052-nsrr.edf</t>
-  </si>
-  <si>
-    <t>chc056-nsrr.edf</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>O1</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>cchin_l</t>
-  </si>
-  <si>
-    <t>ECG1_2</t>
-  </si>
-  <si>
-    <t>spo2</t>
-  </si>
-  <si>
-    <t>flow</t>
-  </si>
-  <si>
-    <t>nas_pres</t>
-  </si>
-  <si>
-    <t>thorax</t>
-  </si>
-  <si>
-    <t>abdomen</t>
-  </si>
-  <si>
-    <t>snore</t>
-  </si>
-  <si>
-    <t>lleg</t>
-  </si>
-  <si>
-    <t>rleg</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>cs_EEG</t>
-  </si>
-  <si>
-    <t>cs_LOC</t>
-  </si>
-  <si>
-    <t>cs_ROC</t>
-  </si>
-  <si>
-    <t>cs_EMG</t>
-  </si>
-  <si>
-    <t>cs_ECG</t>
+    <t>chc001-nsrr</t>
+  </si>
+  <si>
+    <t>chc004-nsrr</t>
+  </si>
+  <si>
+    <t>chc005-nsrr</t>
+  </si>
+  <si>
+    <t>chc006-nsrr</t>
+  </si>
+  <si>
+    <t>chc008-nsrr</t>
+  </si>
+  <si>
+    <t>chc009-nsrr</t>
+  </si>
+  <si>
+    <t>chc010-nsrr</t>
+  </si>
+  <si>
+    <t>chc012-nsrr</t>
+  </si>
+  <si>
+    <t>chc013-nsrr</t>
+  </si>
+  <si>
+    <t>chc014-nsrr</t>
+  </si>
+  <si>
+    <t>chc015-nsrr</t>
+  </si>
+  <si>
+    <t>chc016-nsrr</t>
+  </si>
+  <si>
+    <t>chc022-nsrr</t>
+  </si>
+  <si>
+    <t>chc025-nsrr</t>
+  </si>
+  <si>
+    <t>chc027-nsrr</t>
+  </si>
+  <si>
+    <t>chc028-nsrr</t>
+  </si>
+  <si>
+    <t>chc033-nsrr</t>
+  </si>
+  <si>
+    <t>chc035-nsrr</t>
+  </si>
+  <si>
+    <t>chc037-nsrr</t>
+  </si>
+  <si>
+    <t>chc040-nsrr</t>
+  </si>
+  <si>
+    <t>chc041-nsrr</t>
+  </si>
+  <si>
+    <t>chc052-nsrr</t>
+  </si>
+  <si>
+    <t>chc056-nsrr</t>
+  </si>
+  <si>
+    <t>E1: 128</t>
+  </si>
+  <si>
+    <t>E2: 128</t>
+  </si>
+  <si>
+    <t>F3: 128</t>
+  </si>
+  <si>
+    <t>F4: 128</t>
+  </si>
+  <si>
+    <t>C3: 128</t>
+  </si>
+  <si>
+    <t>C4: 128</t>
+  </si>
+  <si>
+    <t>O1: 128</t>
+  </si>
+  <si>
+    <t>O2: 128</t>
+  </si>
+  <si>
+    <t>cchin_l: 256</t>
+  </si>
+  <si>
+    <t>ECG1_2: 128</t>
+  </si>
+  <si>
+    <t>spo2: 16</t>
+  </si>
+  <si>
+    <t>flow: 32</t>
+  </si>
+  <si>
+    <t>nas_pres: 64</t>
+  </si>
+  <si>
+    <t>thorax: 32</t>
+  </si>
+  <si>
+    <t>abdomen: 32</t>
+  </si>
+  <si>
+    <t>snore: 256</t>
+  </si>
+  <si>
+    <t>lleg: 128</t>
+  </si>
+  <si>
+    <t>rleg: 128</t>
+  </si>
+  <si>
+    <t>position: 16</t>
+  </si>
+  <si>
+    <t>cs_EEG: 100</t>
+  </si>
+  <si>
+    <t>cs_LOC: 100</t>
+  </si>
+  <si>
+    <t>cs_ROC: 100</t>
+  </si>
+  <si>
+    <t>cs_EMG: 100</t>
+  </si>
+  <si>
+    <t>cs_ECG: 100</t>
   </si>
 </sst>
 </file>
@@ -537,10 +537,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="24" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -2392,6 +2396,5 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
record setting(12): chc(1), chp(11)
</commit_message>
<xml_diff>
--- a/log/channel/cnc_chc.xlsx
+++ b/log/channel/cnc_chc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92a996cea29e9e70/future/复旦/信息学院/课题组/narcolepsy_night/narcolepsy_night_code/log/channel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_EAF872967FBACC58567B142B27D06862DC7B69B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06D9D854-1C4D-4E1F-AD99-967034CA15D2}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="109_{69F8A779-E2B1-4421-9591-52FE17C3D494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7EC5F96-D67B-4CA3-88B0-5EB99C183C1F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16200" yWindow="7208" windowWidth="16200" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,12 +189,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -224,10 +230,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -257,34 +267,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -531,13 +541,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -621,73 +631,73 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -695,73 +705,73 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -769,73 +779,73 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -843,73 +853,73 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="X5" t="s">
+      <c r="X5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -917,73 +927,73 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U6" t="s">
+      <c r="U6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V6" t="s">
+      <c r="V6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -991,73 +1001,73 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="X7" t="s">
+      <c r="X7" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1065,73 +1075,73 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X8" t="s">
+      <c r="X8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1139,73 +1149,73 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1213,73 +1223,73 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="X10" t="s">
+      <c r="X10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1287,73 +1297,73 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X11" t="s">
+      <c r="X11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1361,73 +1371,73 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="X12" t="s">
+      <c r="X12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1435,73 +1445,73 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V13" t="s">
+      <c r="V13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X13" t="s">
+      <c r="X13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1509,73 +1519,73 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="V14" t="s">
+      <c r="V14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="X14" t="s">
+      <c r="X14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1583,73 +1593,73 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V15" t="s">
+      <c r="V15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="W15" t="s">
+      <c r="W15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="X15" t="s">
+      <c r="X15" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1657,73 +1667,73 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="V16" t="s">
+      <c r="V16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="W16" t="s">
+      <c r="W16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X16" t="s">
+      <c r="X16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1731,73 +1741,73 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="V17" t="s">
+      <c r="V17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X17" t="s">
+      <c r="X17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1805,73 +1815,73 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S18" t="s">
+      <c r="S18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="V18" t="s">
+      <c r="V18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W18" t="s">
+      <c r="W18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="X18" t="s">
+      <c r="X18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1879,73 +1889,73 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S19" t="s">
+      <c r="S19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U19" t="s">
+      <c r="U19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V19" t="s">
+      <c r="V19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="W19" t="s">
+      <c r="W19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X19" t="s">
+      <c r="X19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1953,73 +1963,73 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U20" t="s">
+      <c r="U20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="W20" t="s">
+      <c r="W20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="X20" t="s">
+      <c r="X20" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2027,73 +2037,73 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S21" t="s">
+      <c r="S21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T21" t="s">
+      <c r="T21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U21" t="s">
+      <c r="U21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W21" t="s">
+      <c r="W21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="X21" t="s">
+      <c r="X21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2101,73 +2111,73 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T22" t="s">
+      <c r="T22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U22" t="s">
+      <c r="U22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V22" t="s">
+      <c r="V22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W22" t="s">
+      <c r="W22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X22" t="s">
+      <c r="X22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2175,73 +2185,73 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S23" t="s">
+      <c r="S23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="T23" t="s">
+      <c r="T23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U23" t="s">
+      <c r="U23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="W23" t="s">
+      <c r="W23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="X23" t="s">
+      <c r="X23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2249,73 +2259,73 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S24" t="s">
+      <c r="S24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="T24" t="s">
+      <c r="T24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="U24" t="s">
+      <c r="U24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="V24" t="s">
+      <c r="V24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="X24" t="s">
+      <c r="X24" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2323,74 +2333,145 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="T25" t="s">
+      <c r="T25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="U25" t="s">
+      <c r="U25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="V25" t="s">
+      <c r="V25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="W25" t="s">
+      <c r="W25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X25" t="s">
+      <c r="X25" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>0</v>
+      </c>
+      <c r="R27" s="3">
+        <v>0</v>
+      </c>
+      <c r="S27" s="3">
+        <v>0</v>
+      </c>
+      <c r="T27" s="3">
+        <v>0</v>
+      </c>
+      <c r="U27" s="3">
+        <v>0</v>
+      </c>
+      <c r="V27" s="3">
+        <v>0</v>
+      </c>
+      <c r="W27" s="3">
+        <v>0</v>
+      </c>
+      <c r="X27" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>